<commit_message>
add correct scoresheet to repo
</commit_message>
<xml_diff>
--- a/CSE316-S25-Project-TestCases.xlsx
+++ b/CSE316-S25-Project-TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AD\project_grading\teams\project-s25-sasha-david-and\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AD\project_grading\teams\project-s25-sharanya-and-fahim-finale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B88E772-FA9C-4EB2-A06F-131A9255477F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DEA59C-0092-45F6-9D08-FD6289D337E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="295">
   <si>
     <t>Assignment:</t>
   </si>
@@ -56,19 +56,19 @@
     <t>Team Name:</t>
   </si>
   <si>
-    <t>Sasha David and</t>
+    <t>sharanya and fahim Finale</t>
   </si>
   <si>
     <t>Student 1:</t>
   </si>
   <si>
-    <t>Alexander Joukov</t>
+    <t>Fahim Jawad</t>
   </si>
   <si>
     <t>Student 2:</t>
   </si>
   <si>
-    <t>David Lai</t>
+    <t>Sharanya Kataru</t>
   </si>
   <si>
     <t>Grader Name:</t>
@@ -931,20 +931,13 @@
     <t>Total[190 pts.]:</t>
   </si>
   <si>
-    <t>was able to create two identical accounts</t>
-  </si>
-  <si>
-    <t>No error reported in client</t>
-  </si>
-  <si>
-    <t>Misc. Penalties</t>
-  </si>
-  <si>
-    <t>view count updates not showing up in browser properly.
-Significant synchronization issues between multiple sessions in different browser instances; cannot trigger update of local data through navigation</t>
-  </si>
-  <si>
-    <t>no zero users message</t>
+    <t>not default listing</t>
+  </si>
+  <si>
+    <t>can't empty listing since admin included, no message about 0 regular users</t>
+  </si>
+  <si>
+    <t>crash on delete of newly created user, failed to remove communities user had created</t>
   </si>
 </sst>
 </file>
@@ -1444,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
@@ -1459,7 +1452,7 @@
     <col min="4" max="4" width="60.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.453125" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.90625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="8.90625" style="2"/>
   </cols>
@@ -1837,12 +1830,10 @@
         <v>64</v>
       </c>
       <c r="E27" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="5"/>
-      <c r="G27" s="5" t="s">
-        <v>292</v>
-      </c>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18"/>
@@ -2030,12 +2021,10 @@
         <v>94</v>
       </c>
       <c r="E38" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="5" t="s">
-        <v>293</v>
-      </c>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
@@ -3815,10 +3804,12 @@
         <v>262</v>
       </c>
       <c r="E141" s="8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F141" s="5"/>
-      <c r="G141" s="5"/>
+      <c r="G141" s="5" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="142" spans="1:7" s="7" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="17"/>
@@ -3866,10 +3857,12 @@
         <v>271</v>
       </c>
       <c r="E144" s="8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F144" s="5"/>
-      <c r="G144" s="5"/>
+      <c r="G144" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="145" spans="1:7" s="7" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="17"/>
@@ -3904,7 +3897,7 @@
       </c>
       <c r="F146" s="5"/>
       <c r="G146" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
@@ -3919,7 +3912,7 @@
       </c>
       <c r="B148" s="13">
         <f>SUM(E11:E146)</f>
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
@@ -3953,7 +3946,7 @@
       </c>
       <c r="B153" s="13">
         <f>SUM(B148,B150,B151)</f>
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
@@ -3988,7 +3981,7 @@
       </c>
       <c r="B158" s="13">
         <f>SUM(B153,B155,B156)</f>
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
@@ -4005,7 +3998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="3" t="s">
         <v>287</v>
       </c>
@@ -4013,7 +4006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="s">
         <v>288</v>
       </c>
@@ -4021,26 +4014,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="3" t="s">
         <v>289</v>
       </c>
       <c r="B164" s="13">
         <f>SUM(B158, B160,B161,B162)</f>
-        <v>183</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
         <v>290</v>
       </c>
@@ -4048,33 +4041,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="s">
         <v>291</v>
       </c>
       <c r="B168" s="13">
-        <f>SUM(B164,B166, B170)</f>
-        <v>180</v>
+        <f>SUM(B164,B166)</f>
+        <v>188</v>
       </c>
       <c r="C168" s="2">
         <f>((B168/190)*100)</f>
-        <v>94.73684210526315</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A170" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="B170" s="2">
-        <v>-7</v>
-      </c>
-      <c r="G170" s="2" t="s">
-        <v>295</v>
+        <v>98.94736842105263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>